<commit_message>
Implemented new scripts and mapping based on discovered service
</commit_message>
<xml_diff>
--- a/migrations/fixtures/exploits.xlsx
+++ b/migrations/fixtures/exploits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="144" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="204" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="95">
   <si>
     <t>app</t>
   </si>
@@ -41,7 +41,7 @@
     <t>SSL POODLE information leak</t>
   </si>
   <si>
-    <t> The SSL protocol 3.0, as used in OpenSSL through 1.0.1i and  other products, uses nondeterministic CBC padding, which makes it easier  for man-in-the-middle attackers to obtain cleartext data via a  padding-oracle attack, aka the "POODLE" issue.</t>
+    <t>The SSL protocol 3.0, as used in OpenSSL through 1.0.1i and  other products, uses nondeterministic CBC padding, which makes it easier  for man-in-the-middle attackers to obtain cleartext data via a  padding-oracle attack, aka the "POODLE" issue.</t>
   </si>
   <si>
     <t>Medium</t>
@@ -95,6 +95,15 @@
     <t>vsFTPd version 2.3.4 backdoor, this was reported on 2011-07-04.</t>
   </si>
   <si>
+    <t>ftp-anon</t>
+  </si>
+  <si>
+    <t>Anonymous FTP login allowed (FTP code 230)</t>
+  </si>
+  <si>
+    <t>Checks if an FTP server allows anonymous logins. If anonymous is allowed, gets a directory listing of the root directory and highlights writeable files.</t>
+  </si>
+  <si>
     <t>distcc-cve2004-2687</t>
   </si>
   <si>
@@ -110,7 +119,187 @@
     <t>RMI registry default configuration remote code execution vulnerability</t>
   </si>
   <si>
-    <t> Default configuration of RMI registry allows loading classes from remote URLs which can lead to remote code executeion.</t>
+    <t>Default configuration of RMI registry allows loading classes from remote URLs which can lead to remote code executeion.</t>
+  </si>
+  <si>
+    <t>smb-vuln-cve2009-3103</t>
+  </si>
+  <si>
+    <t>SMBv2 exploit (CVE-2009-3103, Microsoft Security Advisory 975497)</t>
+  </si>
+  <si>
+    <t>Array index error in the SMBv2 protocol implementation in srv2.sys in Microsoft Windows Vista Gold, SP1, and SP2, Windows Server 2008 Gold and SP2, and Windows 7 RC allows remote attackers to execute arbitrary code or cause a denial of service (system crash) via an &amp; (ampersand) character in a Process ID High header field in a NEGOTIATE PROTOCOL REQUEST packet, which triggers an attempted dereference of an out-of-bounds memory location, aka "SMBv2 Negotiation Vulnerability."</t>
+  </si>
+  <si>
+    <t>http-vuln-cve2014-2127</t>
+  </si>
+  <si>
+    <t>Cisco ASA SSL VPN Privilege Escalation Vulnerability</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance (ASA) Software 8.x before 8.2(5.48), 8.3 before 8.3(2.40), 8.4 before 8.4(7.9), 8.6 before 8.6(1.13), 9.0 before 9.0(4.1), and 9.1 before 9.1(4.3) does not properly process management-session information during privilege validation for SSL VPN portal connections, which allows remote authenticated users to gain privileges by establishing a Clientless SSL VPN session and entering crafted URLs, aka Bug ID CSCul70099.</t>
+  </si>
+  <si>
+    <t>http-vuln-cve2014-2129</t>
+  </si>
+  <si>
+    <t>Cisco ASA SIP Denial of Service Vulnerability</t>
+  </si>
+  <si>
+    <t>The SIP inspection engine in Cisco Adaptive Security Appliance (ASA) Software 8.2 before 8.2(5.48), 8.4 before 8.4(6.5), 9.0 before 9.0(3.1), and 9.1 before 9.1(2.5) allows remote attackers to cause a denial of service (memory consumption or device reload) via crafted SIP packets, aka Bug ID CSCuh44052.</t>
+  </si>
+  <si>
+    <t>http-vuln-cve2014-2126</t>
+  </si>
+  <si>
+    <t>Cisco ASA ASDM Privilege Escalation Vulnerability</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance (ASA) Software 8.2 before 8.2(5.47), 8.4 before 8.4(7.5), 8.7 before 8.7(1.11), 9.0 before 9.0(3.10), and 9.1 before 9.1(3.4) allows remote authenticated users to gain privileges by leveraging level-0 ASDM access, aka Bug ID CSCuj33496.</t>
+  </si>
+  <si>
+    <t>http-vuln-cve2015-1635</t>
+  </si>
+  <si>
+    <t>Remote Code Execution in HTTP.sys (MS15-034)</t>
+  </si>
+  <si>
+    <t>A remote code execution vulnerability exists in the HTTP protocol stack (HTTP.sys) that is caused when HTTP.sys improperly parses specially crafted HTTP requests. An attacker who successfully exploited this vulnerability could execute arbitrary code in the context of the System account.</t>
+  </si>
+  <si>
+    <t>http-vuln-cve2015-1427</t>
+  </si>
+  <si>
+    <t>ElasticSearch CVE-2015-1427 RCE Exploit</t>
+  </si>
+  <si>
+    <t>The vulnerability allows an attacker to construct Groovy scripts that escape the sandbox and execute shell commands as the user running the Elasticsearch Java VM.</t>
+  </si>
+  <si>
+    <t>irc-unrealircd-backdoor</t>
+  </si>
+  <si>
+    <t>Checks IRC backdoor</t>
+  </si>
+  <si>
+    <t>Checks if an IRC server is backdoored by running a time-based command (ping) and checking how long it takes to respond.</t>
+  </si>
+  <si>
+    <t>iscsi-info</t>
+  </si>
+  <si>
+    <t>Collects and displays information from remote iSCSI targets</t>
+  </si>
+  <si>
+    <t>Collects and displays information from remote iSCSI targets.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>ssh2-enum-algos</t>
+  </si>
+  <si>
+    <t>SSH2 algorithms</t>
+  </si>
+  <si>
+    <t>Reports the number of algorithms (for encryption, compression, etc.) that the target SSH2 server offers. If verbosity is set, the offered algorithms are each listed by type. If the "client to server" and "server to client" algorithm lists are identical (order specifies preference) then the list is shown only once under a combined type.</t>
+  </si>
+  <si>
+    <t>ssh-hostkey</t>
+  </si>
+  <si>
+    <t>SSH hostkeys</t>
+  </si>
+  <si>
+    <t>Shows SSH hostkeys. Shows the target SSH server's key fingerprint and the public key itself.</t>
+  </si>
+  <si>
+    <t>smb-os-discovery</t>
+  </si>
+  <si>
+    <t>SMB information</t>
+  </si>
+  <si>
+    <t>Attempts to determine the operating system, computer name, domain, workgroup, and current  time over the SMB protocol (ports 445 or 139). This is done by starting a session with the anonymous account (or with a proper user account, if one is given; it likely doesn't make a difference); in response to a session starting, the server will send back all this information.</t>
+  </si>
+  <si>
+    <t>mysql-info</t>
+  </si>
+  <si>
+    <t>MySQL information</t>
+  </si>
+  <si>
+    <t>Connects to a MySQL server and prints information such as the protocol and version numbers, thread ID, status, capabilities, and the password salt.</t>
+  </si>
+  <si>
+    <t>mongodb-databases</t>
+  </si>
+  <si>
+    <t>MongoDB databases</t>
+  </si>
+  <si>
+    <t>Attempts to get a list of tables from a MongoDB database.</t>
+  </si>
+  <si>
+    <t>mongodb-info</t>
+  </si>
+  <si>
+    <t>MongoDB information</t>
+  </si>
+  <si>
+    <t>ike-version</t>
+  </si>
+  <si>
+    <t>IKE version</t>
+  </si>
+  <si>
+    <t>Obtains information (such as vendor and device type where available) from an IKE service by sending four packets to the host.  This scripts tests with both Main and Aggressive Mode and sends multiple transforms per request.</t>
+  </si>
+  <si>
+    <t>ldap-search</t>
+  </si>
+  <si>
+    <t>LDAP search</t>
+  </si>
+  <si>
+    <t>Attempts to perform an LDAP search and returns all matches.</t>
+  </si>
+  <si>
+    <t>http-enum</t>
+  </si>
+  <si>
+    <t>HTTP enumeration</t>
+  </si>
+  <si>
+    <t>Enumerates directories used by popular web applications and servers.</t>
+  </si>
+  <si>
+    <t>http-php-version</t>
+  </si>
+  <si>
+    <t>HTTP PHP version</t>
+  </si>
+  <si>
+    <t>Attempts to retrieve the PHP version from a web server.</t>
+  </si>
+  <si>
+    <t>vnc-info</t>
+  </si>
+  <si>
+    <t>VNC information</t>
+  </si>
+  <si>
+    <t>Queries a VNC server for its protocol version and supported security types.</t>
+  </si>
+  <si>
+    <t>rpcinfo</t>
+  </si>
+  <si>
+    <t>RPC information</t>
+  </si>
+  <si>
+    <t>Connects to portmapper and fetches a list of all registered programs.  It then prints out a table including (for each program) the RPC program number, supported version numbers, port number and protocol, and program name.</t>
   </si>
 </sst>
 </file>
@@ -125,6 +314,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -147,6 +337,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -283,16 +474,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.0765306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.6020408163265"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.0969387755102"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
@@ -448,6 +640,363 @@
       </c>
       <c r="E9" s="0" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>